<commit_message>
updated extent report for adding failed steps
</commit_message>
<xml_diff>
--- a/testng-excel-extentreport/src/test/resources/ExpediaTestData.xlsx
+++ b/testng-excel-extentreport/src/test/resources/ExpediaTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Origin</t>
   </si>
@@ -40,24 +40,12 @@
     <t>London, United Kingdom (LHR-Heathrow)</t>
   </si>
   <si>
-    <t>26/05/2019</t>
-  </si>
-  <si>
     <t>SNO</t>
   </si>
   <si>
-    <t>30/05/2019</t>
-  </si>
-  <si>
     <t>Venice, Italy (VCE-Marco Polo)</t>
   </si>
   <si>
-    <t>20/06/2019</t>
-  </si>
-  <si>
-    <t>01/07/2019</t>
-  </si>
-  <si>
     <t>Mumbai, India (BOM-Chhatrapati Shivaji Intl.)</t>
   </si>
   <si>
@@ -68,6 +56,24 @@
   </si>
   <si>
     <t>Liverpool, United Kingdom (LPL-John Lennon)</t>
+  </si>
+  <si>
+    <t>26/08/2019</t>
+  </si>
+  <si>
+    <t>30/10/2019</t>
+  </si>
+  <si>
+    <t>20/08/2019</t>
+  </si>
+  <si>
+    <t>01/10/2019</t>
+  </si>
+  <si>
+    <t>30/11/2019</t>
+  </si>
+  <si>
+    <t>01/11/2019</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,7 +406,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,7 +419,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -439,10 +445,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -453,13 +459,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +479,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,7 +492,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -506,16 +512,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -523,16 +529,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>